<commit_message>
add 1.point0-100 2.IdDuplicationCheck 3.Id&PointIntegerCheck
</commit_message>
<xml_diff>
--- a/studentGrades.xlsx
+++ b/studentGrades.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Geography Grades" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Physics Grades" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,31 +454,17 @@
       <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B2" t="n">
+        <v>123</v>
+      </c>
+      <c r="C2" t="inlineStr">
         <is>
-          <t>123</t>
+          <t>F</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Pass</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>123</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Pass</t>
+          <t>Fail</t>
         </is>
       </c>
     </row>

</xml_diff>